<commit_message>
processing file, showing not found regions and inserting data to database in browser (15.06.2024)
</commit_message>
<xml_diff>
--- a/Hello.xlsx
+++ b/Hello.xlsx
@@ -53,11 +53,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -435,7 +432,7 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="5">
-      <c r="D5" s="2" t="inlineStr">
+      <c r="D5" s="1" t="inlineStr">
         <is>
           <t>SOS</t>
         </is>

</xml_diff>